<commit_message>
Fix Gemini answer handling for list type; update system prompt citation format
- Handle cases where Gemini model returns a list for answer content, preventing attribute errors.
- Add a visual separator before each question prompt in CLI.
- Update citation format in system
</commit_message>
<xml_diff>
--- a/document/excel/Employee List.xlsx
+++ b/document/excel/Employee List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Project\rag\document\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF66F8EC-D4A3-4DF3-B4BA-09475A22ED3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EA126-34C0-474C-86E6-E6E6EC859537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4380" yWindow="-13068" windowWidth="30936" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="2381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4052" uniqueCount="2389">
   <si>
     <t>STT</t>
   </si>
@@ -7163,6 +7163,30 @@
   </si>
   <si>
     <t>898.540.1926x7489</t>
+  </si>
+  <si>
+    <t>NV0401</t>
+  </si>
+  <si>
+    <t>Lis Johnson</t>
+  </si>
+  <si>
+    <t>NV0402</t>
+  </si>
+  <si>
+    <t>Carhol Deleon</t>
+  </si>
+  <si>
+    <t>NV0403</t>
+  </si>
+  <si>
+    <t>NV0404</t>
+  </si>
+  <si>
+    <t>Lis Torrest</t>
+  </si>
+  <si>
+    <t>Jeremy Griffin</t>
   </si>
 </sst>
 </file>
@@ -7531,26 +7555,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L401"/>
+  <dimension ref="A1:L405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="A402" sqref="A402:XFD499"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7588,7 +7612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -7624,7 +7648,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -7660,7 +7684,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -7696,7 +7720,7 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -7732,7 +7756,7 @@
       </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -7768,7 +7792,7 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -7804,7 +7828,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -7840,7 +7864,7 @@
       </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -7876,7 +7900,7 @@
       </c>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -7912,7 +7936,7 @@
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -7948,7 +7972,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -7984,7 +8008,7 @@
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -8020,7 +8044,7 @@
       </c>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -8056,7 +8080,7 @@
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -8092,7 +8116,7 @@
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -8128,7 +8152,7 @@
       </c>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -8164,7 +8188,7 @@
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -8200,7 +8224,7 @@
       </c>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -8236,7 +8260,7 @@
       </c>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -8272,7 +8296,7 @@
       </c>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -8308,7 +8332,7 @@
       </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -8344,7 +8368,7 @@
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -8380,7 +8404,7 @@
       </c>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -8416,7 +8440,7 @@
       </c>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -8452,7 +8476,7 @@
       </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -8488,7 +8512,7 @@
       </c>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -8524,7 +8548,7 @@
       </c>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -8560,7 +8584,7 @@
       </c>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -8596,7 +8620,7 @@
       </c>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -8632,7 +8656,7 @@
       </c>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -8668,7 +8692,7 @@
       </c>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -8704,7 +8728,7 @@
       </c>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -8740,7 +8764,7 @@
       </c>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -8776,7 +8800,7 @@
       </c>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -8812,7 +8836,7 @@
       </c>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -8848,7 +8872,7 @@
       </c>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -8884,7 +8908,7 @@
       </c>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -8920,7 +8944,7 @@
       </c>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -8956,7 +8980,7 @@
       </c>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -8992,7 +9016,7 @@
       </c>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -9028,7 +9052,7 @@
       </c>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -9064,7 +9088,7 @@
       </c>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -9100,7 +9124,7 @@
       </c>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -9136,7 +9160,7 @@
       </c>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -9172,7 +9196,7 @@
       </c>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -9208,7 +9232,7 @@
       </c>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -9244,7 +9268,7 @@
       </c>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -9280,7 +9304,7 @@
       </c>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -9316,7 +9340,7 @@
       </c>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -9352,7 +9376,7 @@
       </c>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -9388,7 +9412,7 @@
       </c>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -9424,7 +9448,7 @@
       </c>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -9460,7 +9484,7 @@
       </c>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -9496,7 +9520,7 @@
       </c>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -9532,7 +9556,7 @@
       </c>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -9568,7 +9592,7 @@
       </c>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -9604,7 +9628,7 @@
       </c>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -9640,7 +9664,7 @@
       </c>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -9676,7 +9700,7 @@
       </c>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -9712,7 +9736,7 @@
       </c>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -9748,7 +9772,7 @@
       </c>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -9784,7 +9808,7 @@
       </c>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -9820,7 +9844,7 @@
       </c>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -9856,7 +9880,7 @@
       </c>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -9892,7 +9916,7 @@
       </c>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -9928,7 +9952,7 @@
       </c>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -9964,7 +9988,7 @@
       </c>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -10000,7 +10024,7 @@
       </c>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -10036,7 +10060,7 @@
       </c>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -10072,7 +10096,7 @@
       </c>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -10108,7 +10132,7 @@
       </c>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -10144,7 +10168,7 @@
       </c>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -10180,7 +10204,7 @@
       </c>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -10216,7 +10240,7 @@
       </c>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -10252,7 +10276,7 @@
       </c>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -10288,7 +10312,7 @@
       </c>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -10324,7 +10348,7 @@
       </c>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -10360,7 +10384,7 @@
       </c>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -10396,7 +10420,7 @@
       </c>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -10432,7 +10456,7 @@
       </c>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -10468,7 +10492,7 @@
       </c>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -10504,7 +10528,7 @@
       </c>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -10540,7 +10564,7 @@
       </c>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -10576,7 +10600,7 @@
       </c>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -10612,7 +10636,7 @@
       </c>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -10648,7 +10672,7 @@
       </c>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -10684,7 +10708,7 @@
       </c>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -10720,7 +10744,7 @@
       </c>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -10756,7 +10780,7 @@
       </c>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -10792,7 +10816,7 @@
       </c>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -10828,7 +10852,7 @@
       </c>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -10864,7 +10888,7 @@
       </c>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -10900,7 +10924,7 @@
       </c>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -10936,7 +10960,7 @@
       </c>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -10972,7 +10996,7 @@
       </c>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -11008,7 +11032,7 @@
       </c>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -11044,7 +11068,7 @@
       </c>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -11080,7 +11104,7 @@
       </c>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -11116,7 +11140,7 @@
       </c>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -11152,7 +11176,7 @@
       </c>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -11188,7 +11212,7 @@
       </c>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -11224,7 +11248,7 @@
       </c>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -11260,7 +11284,7 @@
       </c>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -11296,7 +11320,7 @@
       </c>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -11332,7 +11356,7 @@
       </c>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -11368,7 +11392,7 @@
       </c>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -11404,7 +11428,7 @@
       </c>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -11440,7 +11464,7 @@
       </c>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -11476,7 +11500,7 @@
       </c>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -11512,7 +11536,7 @@
       </c>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -11548,7 +11572,7 @@
       </c>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -11584,7 +11608,7 @@
       </c>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -11620,7 +11644,7 @@
       </c>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -11656,7 +11680,7 @@
       </c>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -11692,7 +11716,7 @@
       </c>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -11728,7 +11752,7 @@
       </c>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -11764,7 +11788,7 @@
       </c>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -11800,7 +11824,7 @@
       </c>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -11836,7 +11860,7 @@
       </c>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -11872,7 +11896,7 @@
       </c>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -11908,7 +11932,7 @@
       </c>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -11944,7 +11968,7 @@
       </c>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -11980,7 +12004,7 @@
       </c>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -12016,7 +12040,7 @@
       </c>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -12052,7 +12076,7 @@
       </c>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -12088,7 +12112,7 @@
       </c>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -12124,7 +12148,7 @@
       </c>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -12160,7 +12184,7 @@
       </c>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -12196,7 +12220,7 @@
       </c>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -12232,7 +12256,7 @@
       </c>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -12268,7 +12292,7 @@
       </c>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -12304,7 +12328,7 @@
       </c>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -12340,7 +12364,7 @@
       </c>
       <c r="L133" s="2"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -12376,7 +12400,7 @@
       </c>
       <c r="L134" s="2"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -12412,7 +12436,7 @@
       </c>
       <c r="L135" s="2"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -12448,7 +12472,7 @@
       </c>
       <c r="L136" s="2"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -12484,7 +12508,7 @@
       </c>
       <c r="L137" s="2"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -12520,7 +12544,7 @@
       </c>
       <c r="L138" s="2"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -12556,7 +12580,7 @@
       </c>
       <c r="L139" s="2"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -12592,7 +12616,7 @@
       </c>
       <c r="L140" s="2"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -12628,7 +12652,7 @@
       </c>
       <c r="L141" s="2"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -12664,7 +12688,7 @@
       </c>
       <c r="L142" s="2"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -12700,7 +12724,7 @@
       </c>
       <c r="L143" s="2"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -12736,7 +12760,7 @@
       </c>
       <c r="L144" s="2"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -12772,7 +12796,7 @@
       </c>
       <c r="L145" s="2"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -12808,7 +12832,7 @@
       </c>
       <c r="L146" s="2"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -12844,7 +12868,7 @@
       </c>
       <c r="L147" s="2"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -12880,7 +12904,7 @@
       </c>
       <c r="L148" s="2"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -12916,7 +12940,7 @@
       </c>
       <c r="L149" s="2"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -12952,7 +12976,7 @@
       </c>
       <c r="L150" s="2"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -12988,7 +13012,7 @@
       </c>
       <c r="L151" s="2"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -13024,7 +13048,7 @@
       </c>
       <c r="L152" s="2"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -13060,7 +13084,7 @@
       </c>
       <c r="L153" s="2"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -13096,7 +13120,7 @@
       </c>
       <c r="L154" s="2"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -13132,7 +13156,7 @@
       </c>
       <c r="L155" s="2"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -13168,7 +13192,7 @@
       </c>
       <c r="L156" s="2"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -13204,7 +13228,7 @@
       </c>
       <c r="L157" s="2"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -13240,7 +13264,7 @@
       </c>
       <c r="L158" s="2"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -13276,7 +13300,7 @@
       </c>
       <c r="L159" s="2"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -13312,7 +13336,7 @@
       </c>
       <c r="L160" s="2"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -13348,7 +13372,7 @@
       </c>
       <c r="L161" s="2"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -13384,7 +13408,7 @@
       </c>
       <c r="L162" s="2"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -13420,7 +13444,7 @@
       </c>
       <c r="L163" s="2"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -13456,7 +13480,7 @@
       </c>
       <c r="L164" s="2"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -13492,7 +13516,7 @@
       </c>
       <c r="L165" s="2"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -13528,7 +13552,7 @@
       </c>
       <c r="L166" s="2"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -13564,7 +13588,7 @@
       </c>
       <c r="L167" s="2"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -13600,7 +13624,7 @@
       </c>
       <c r="L168" s="2"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -13636,7 +13660,7 @@
       </c>
       <c r="L169" s="2"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -13672,7 +13696,7 @@
       </c>
       <c r="L170" s="2"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -13708,7 +13732,7 @@
       </c>
       <c r="L171" s="2"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -13744,7 +13768,7 @@
       </c>
       <c r="L172" s="2"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -13780,7 +13804,7 @@
       </c>
       <c r="L173" s="2"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -13816,7 +13840,7 @@
       </c>
       <c r="L174" s="2"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -13852,7 +13876,7 @@
       </c>
       <c r="L175" s="2"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -13888,7 +13912,7 @@
       </c>
       <c r="L176" s="2"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -13924,7 +13948,7 @@
       </c>
       <c r="L177" s="2"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -13960,7 +13984,7 @@
       </c>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -13996,7 +14020,7 @@
       </c>
       <c r="L179" s="2"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -14032,7 +14056,7 @@
       </c>
       <c r="L180" s="2"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -14068,7 +14092,7 @@
       </c>
       <c r="L181" s="2"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -14104,7 +14128,7 @@
       </c>
       <c r="L182" s="2"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -14140,7 +14164,7 @@
       </c>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -14176,7 +14200,7 @@
       </c>
       <c r="L184" s="2"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -14212,7 +14236,7 @@
       </c>
       <c r="L185" s="2"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -14248,7 +14272,7 @@
       </c>
       <c r="L186" s="2"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -14284,7 +14308,7 @@
       </c>
       <c r="L187" s="2"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -14320,7 +14344,7 @@
       </c>
       <c r="L188" s="2"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -14356,7 +14380,7 @@
       </c>
       <c r="L189" s="2"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -14392,7 +14416,7 @@
       </c>
       <c r="L190" s="2"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -14428,7 +14452,7 @@
       </c>
       <c r="L191" s="2"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -14464,7 +14488,7 @@
       </c>
       <c r="L192" s="2"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -14500,7 +14524,7 @@
       </c>
       <c r="L193" s="2"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -14536,7 +14560,7 @@
       </c>
       <c r="L194" s="2"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -14572,7 +14596,7 @@
       </c>
       <c r="L195" s="2"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -14608,7 +14632,7 @@
       </c>
       <c r="L196" s="2"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -14644,7 +14668,7 @@
       </c>
       <c r="L197" s="2"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -14680,7 +14704,7 @@
       </c>
       <c r="L198" s="2"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -14716,7 +14740,7 @@
       </c>
       <c r="L199" s="2"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -14752,7 +14776,7 @@
       </c>
       <c r="L200" s="2"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -14788,7 +14812,7 @@
       </c>
       <c r="L201" s="2"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -14824,7 +14848,7 @@
       </c>
       <c r="L202" s="2"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -14860,7 +14884,7 @@
       </c>
       <c r="L203" s="2"/>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -14896,7 +14920,7 @@
       </c>
       <c r="L204" s="2"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -14932,7 +14956,7 @@
       </c>
       <c r="L205" s="2"/>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -14968,7 +14992,7 @@
       </c>
       <c r="L206" s="2"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <v>206</v>
       </c>
@@ -15004,7 +15028,7 @@
       </c>
       <c r="L207" s="2"/>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>207</v>
       </c>
@@ -15040,7 +15064,7 @@
       </c>
       <c r="L208" s="2"/>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -15076,7 +15100,7 @@
       </c>
       <c r="L209" s="2"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -15112,7 +15136,7 @@
       </c>
       <c r="L210" s="2"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -15148,7 +15172,7 @@
       </c>
       <c r="L211" s="2"/>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -15184,7 +15208,7 @@
       </c>
       <c r="L212" s="2"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -15220,7 +15244,7 @@
       </c>
       <c r="L213" s="2"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -15256,7 +15280,7 @@
       </c>
       <c r="L214" s="2"/>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -15292,7 +15316,7 @@
       </c>
       <c r="L215" s="2"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -15328,7 +15352,7 @@
       </c>
       <c r="L216" s="2"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -15364,7 +15388,7 @@
       </c>
       <c r="L217" s="2"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -15400,7 +15424,7 @@
       </c>
       <c r="L218" s="2"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -15436,7 +15460,7 @@
       </c>
       <c r="L219" s="2"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" s="2">
         <v>219</v>
       </c>
@@ -15472,7 +15496,7 @@
       </c>
       <c r="L220" s="2"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -15508,7 +15532,7 @@
       </c>
       <c r="L221" s="2"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -15544,7 +15568,7 @@
       </c>
       <c r="L222" s="2"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -15580,7 +15604,7 @@
       </c>
       <c r="L223" s="2"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -15616,7 +15640,7 @@
       </c>
       <c r="L224" s="2"/>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -15652,7 +15676,7 @@
       </c>
       <c r="L225" s="2"/>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" s="2">
         <v>225</v>
       </c>
@@ -15688,7 +15712,7 @@
       </c>
       <c r="L226" s="2"/>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227" s="2">
         <v>226</v>
       </c>
@@ -15724,7 +15748,7 @@
       </c>
       <c r="L227" s="2"/>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228" s="2">
         <v>227</v>
       </c>
@@ -15760,7 +15784,7 @@
       </c>
       <c r="L228" s="2"/>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -15796,7 +15820,7 @@
       </c>
       <c r="L229" s="2"/>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" s="2">
         <v>229</v>
       </c>
@@ -15832,7 +15856,7 @@
       </c>
       <c r="L230" s="2"/>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -15868,7 +15892,7 @@
       </c>
       <c r="L231" s="2"/>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232" s="2">
         <v>231</v>
       </c>
@@ -15904,7 +15928,7 @@
       </c>
       <c r="L232" s="2"/>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233" s="2">
         <v>232</v>
       </c>
@@ -15940,7 +15964,7 @@
       </c>
       <c r="L233" s="2"/>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234" s="2">
         <v>233</v>
       </c>
@@ -15976,7 +16000,7 @@
       </c>
       <c r="L234" s="2"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -16012,7 +16036,7 @@
       </c>
       <c r="L235" s="2"/>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -16048,7 +16072,7 @@
       </c>
       <c r="L236" s="2"/>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -16084,7 +16108,7 @@
       </c>
       <c r="L237" s="2"/>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -16120,7 +16144,7 @@
       </c>
       <c r="L238" s="2"/>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239" s="2">
         <v>238</v>
       </c>
@@ -16156,7 +16180,7 @@
       </c>
       <c r="L239" s="2"/>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -16192,7 +16216,7 @@
       </c>
       <c r="L240" s="2"/>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241" s="2">
         <v>240</v>
       </c>
@@ -16228,7 +16252,7 @@
       </c>
       <c r="L241" s="2"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" s="2">
         <v>241</v>
       </c>
@@ -16264,7 +16288,7 @@
       </c>
       <c r="L242" s="2"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -16300,7 +16324,7 @@
       </c>
       <c r="L243" s="2"/>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -16336,7 +16360,7 @@
       </c>
       <c r="L244" s="2"/>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" s="2">
         <v>244</v>
       </c>
@@ -16372,7 +16396,7 @@
       </c>
       <c r="L245" s="2"/>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" s="2">
         <v>245</v>
       </c>
@@ -16408,7 +16432,7 @@
       </c>
       <c r="L246" s="2"/>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" s="2">
         <v>246</v>
       </c>
@@ -16444,7 +16468,7 @@
       </c>
       <c r="L247" s="2"/>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" s="2">
         <v>247</v>
       </c>
@@ -16480,7 +16504,7 @@
       </c>
       <c r="L248" s="2"/>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" s="2">
         <v>248</v>
       </c>
@@ -16516,7 +16540,7 @@
       </c>
       <c r="L249" s="2"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -16552,7 +16576,7 @@
       </c>
       <c r="L250" s="2"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -16588,7 +16612,7 @@
       </c>
       <c r="L251" s="2"/>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" s="2">
         <v>251</v>
       </c>
@@ -16624,7 +16648,7 @@
       </c>
       <c r="L252" s="2"/>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -16660,7 +16684,7 @@
       </c>
       <c r="L253" s="2"/>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -16696,7 +16720,7 @@
       </c>
       <c r="L254" s="2"/>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" s="2">
         <v>254</v>
       </c>
@@ -16732,7 +16756,7 @@
       </c>
       <c r="L255" s="2"/>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" s="2">
         <v>255</v>
       </c>
@@ -16768,7 +16792,7 @@
       </c>
       <c r="L256" s="2"/>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" s="2">
         <v>256</v>
       </c>
@@ -16804,7 +16828,7 @@
       </c>
       <c r="L257" s="2"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" s="2">
         <v>257</v>
       </c>
@@ -16840,7 +16864,7 @@
       </c>
       <c r="L258" s="2"/>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" s="2">
         <v>258</v>
       </c>
@@ -16876,7 +16900,7 @@
       </c>
       <c r="L259" s="2"/>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" s="2">
         <v>259</v>
       </c>
@@ -16912,7 +16936,7 @@
       </c>
       <c r="L260" s="2"/>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -16948,7 +16972,7 @@
       </c>
       <c r="L261" s="2"/>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -16984,7 +17008,7 @@
       </c>
       <c r="L262" s="2"/>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -17020,7 +17044,7 @@
       </c>
       <c r="L263" s="2"/>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -17056,7 +17080,7 @@
       </c>
       <c r="L264" s="2"/>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -17092,7 +17116,7 @@
       </c>
       <c r="L265" s="2"/>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266" s="2">
         <v>265</v>
       </c>
@@ -17128,7 +17152,7 @@
       </c>
       <c r="L266" s="2"/>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267" s="2">
         <v>266</v>
       </c>
@@ -17164,7 +17188,7 @@
       </c>
       <c r="L267" s="2"/>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A268" s="2">
         <v>267</v>
       </c>
@@ -17200,7 +17224,7 @@
       </c>
       <c r="L268" s="2"/>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269" s="2">
         <v>268</v>
       </c>
@@ -17236,7 +17260,7 @@
       </c>
       <c r="L269" s="2"/>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A270" s="2">
         <v>269</v>
       </c>
@@ -17272,7 +17296,7 @@
       </c>
       <c r="L270" s="2"/>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A271" s="2">
         <v>270</v>
       </c>
@@ -17308,7 +17332,7 @@
       </c>
       <c r="L271" s="2"/>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A272" s="2">
         <v>271</v>
       </c>
@@ -17344,7 +17368,7 @@
       </c>
       <c r="L272" s="2"/>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A273" s="2">
         <v>272</v>
       </c>
@@ -17380,7 +17404,7 @@
       </c>
       <c r="L273" s="2"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A274" s="2">
         <v>273</v>
       </c>
@@ -17416,7 +17440,7 @@
       </c>
       <c r="L274" s="2"/>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A275" s="2">
         <v>274</v>
       </c>
@@ -17452,7 +17476,7 @@
       </c>
       <c r="L275" s="2"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A276" s="2">
         <v>275</v>
       </c>
@@ -17488,7 +17512,7 @@
       </c>
       <c r="L276" s="2"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A277" s="2">
         <v>276</v>
       </c>
@@ -17524,7 +17548,7 @@
       </c>
       <c r="L277" s="2"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278" s="2">
         <v>277</v>
       </c>
@@ -17560,7 +17584,7 @@
       </c>
       <c r="L278" s="2"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A279" s="2">
         <v>278</v>
       </c>
@@ -17596,7 +17620,7 @@
       </c>
       <c r="L279" s="2"/>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A280" s="2">
         <v>279</v>
       </c>
@@ -17632,7 +17656,7 @@
       </c>
       <c r="L280" s="2"/>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A281" s="2">
         <v>280</v>
       </c>
@@ -17668,7 +17692,7 @@
       </c>
       <c r="L281" s="2"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282" s="2">
         <v>281</v>
       </c>
@@ -17704,7 +17728,7 @@
       </c>
       <c r="L282" s="2"/>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A283" s="2">
         <v>282</v>
       </c>
@@ -17740,7 +17764,7 @@
       </c>
       <c r="L283" s="2"/>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A284" s="2">
         <v>283</v>
       </c>
@@ -17776,7 +17800,7 @@
       </c>
       <c r="L284" s="2"/>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285" s="2">
         <v>284</v>
       </c>
@@ -17812,7 +17836,7 @@
       </c>
       <c r="L285" s="2"/>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A286" s="2">
         <v>285</v>
       </c>
@@ -17848,7 +17872,7 @@
       </c>
       <c r="L286" s="2"/>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A287" s="2">
         <v>286</v>
       </c>
@@ -17884,7 +17908,7 @@
       </c>
       <c r="L287" s="2"/>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A288" s="2">
         <v>287</v>
       </c>
@@ -17920,7 +17944,7 @@
       </c>
       <c r="L288" s="2"/>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A289" s="2">
         <v>288</v>
       </c>
@@ -17956,7 +17980,7 @@
       </c>
       <c r="L289" s="2"/>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A290" s="2">
         <v>289</v>
       </c>
@@ -17992,7 +18016,7 @@
       </c>
       <c r="L290" s="2"/>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A291" s="2">
         <v>290</v>
       </c>
@@ -18028,7 +18052,7 @@
       </c>
       <c r="L291" s="2"/>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A292" s="2">
         <v>291</v>
       </c>
@@ -18064,7 +18088,7 @@
       </c>
       <c r="L292" s="2"/>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A293" s="2">
         <v>292</v>
       </c>
@@ -18100,7 +18124,7 @@
       </c>
       <c r="L293" s="2"/>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A294" s="2">
         <v>293</v>
       </c>
@@ -18136,7 +18160,7 @@
       </c>
       <c r="L294" s="2"/>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A295" s="2">
         <v>294</v>
       </c>
@@ -18172,7 +18196,7 @@
       </c>
       <c r="L295" s="2"/>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A296" s="2">
         <v>295</v>
       </c>
@@ -18208,7 +18232,7 @@
       </c>
       <c r="L296" s="2"/>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A297" s="2">
         <v>296</v>
       </c>
@@ -18244,7 +18268,7 @@
       </c>
       <c r="L297" s="2"/>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A298" s="2">
         <v>297</v>
       </c>
@@ -18280,7 +18304,7 @@
       </c>
       <c r="L298" s="2"/>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A299" s="2">
         <v>298</v>
       </c>
@@ -18316,7 +18340,7 @@
       </c>
       <c r="L299" s="2"/>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A300" s="2">
         <v>299</v>
       </c>
@@ -18352,7 +18376,7 @@
       </c>
       <c r="L300" s="2"/>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A301" s="2">
         <v>300</v>
       </c>
@@ -18388,7 +18412,7 @@
       </c>
       <c r="L301" s="2"/>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A302" s="2">
         <v>301</v>
       </c>
@@ -18424,7 +18448,7 @@
       </c>
       <c r="L302" s="2"/>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A303" s="2">
         <v>302</v>
       </c>
@@ -18460,7 +18484,7 @@
       </c>
       <c r="L303" s="2"/>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A304" s="2">
         <v>303</v>
       </c>
@@ -18496,7 +18520,7 @@
       </c>
       <c r="L304" s="2"/>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A305" s="2">
         <v>304</v>
       </c>
@@ -18532,7 +18556,7 @@
       </c>
       <c r="L305" s="2"/>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A306" s="2">
         <v>305</v>
       </c>
@@ -18568,7 +18592,7 @@
       </c>
       <c r="L306" s="2"/>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A307" s="2">
         <v>306</v>
       </c>
@@ -18604,7 +18628,7 @@
       </c>
       <c r="L307" s="2"/>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A308" s="2">
         <v>307</v>
       </c>
@@ -18640,7 +18664,7 @@
       </c>
       <c r="L308" s="2"/>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A309" s="2">
         <v>308</v>
       </c>
@@ -18676,7 +18700,7 @@
       </c>
       <c r="L309" s="2"/>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A310" s="2">
         <v>309</v>
       </c>
@@ -18712,7 +18736,7 @@
       </c>
       <c r="L310" s="2"/>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A311" s="2">
         <v>310</v>
       </c>
@@ -18748,7 +18772,7 @@
       </c>
       <c r="L311" s="2"/>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A312" s="2">
         <v>311</v>
       </c>
@@ -18784,7 +18808,7 @@
       </c>
       <c r="L312" s="2"/>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A313" s="2">
         <v>312</v>
       </c>
@@ -18820,7 +18844,7 @@
       </c>
       <c r="L313" s="2"/>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A314" s="2">
         <v>313</v>
       </c>
@@ -18856,7 +18880,7 @@
       </c>
       <c r="L314" s="2"/>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A315" s="2">
         <v>314</v>
       </c>
@@ -18892,7 +18916,7 @@
       </c>
       <c r="L315" s="2"/>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A316" s="2">
         <v>315</v>
       </c>
@@ -18928,7 +18952,7 @@
       </c>
       <c r="L316" s="2"/>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A317" s="2">
         <v>316</v>
       </c>
@@ -18964,7 +18988,7 @@
       </c>
       <c r="L317" s="2"/>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A318" s="2">
         <v>317</v>
       </c>
@@ -19000,7 +19024,7 @@
       </c>
       <c r="L318" s="2"/>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A319" s="2">
         <v>318</v>
       </c>
@@ -19036,7 +19060,7 @@
       </c>
       <c r="L319" s="2"/>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A320" s="2">
         <v>319</v>
       </c>
@@ -19072,7 +19096,7 @@
       </c>
       <c r="L320" s="2"/>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A321" s="2">
         <v>320</v>
       </c>
@@ -19108,7 +19132,7 @@
       </c>
       <c r="L321" s="2"/>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A322" s="2">
         <v>321</v>
       </c>
@@ -19144,7 +19168,7 @@
       </c>
       <c r="L322" s="2"/>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A323" s="2">
         <v>322</v>
       </c>
@@ -19180,7 +19204,7 @@
       </c>
       <c r="L323" s="2"/>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A324" s="2">
         <v>323</v>
       </c>
@@ -19216,7 +19240,7 @@
       </c>
       <c r="L324" s="2"/>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A325" s="2">
         <v>324</v>
       </c>
@@ -19252,7 +19276,7 @@
       </c>
       <c r="L325" s="2"/>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A326" s="2">
         <v>325</v>
       </c>
@@ -19288,7 +19312,7 @@
       </c>
       <c r="L326" s="2"/>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A327" s="2">
         <v>326</v>
       </c>
@@ -19324,7 +19348,7 @@
       </c>
       <c r="L327" s="2"/>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A328" s="2">
         <v>327</v>
       </c>
@@ -19360,7 +19384,7 @@
       </c>
       <c r="L328" s="2"/>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A329" s="2">
         <v>328</v>
       </c>
@@ -19396,7 +19420,7 @@
       </c>
       <c r="L329" s="2"/>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A330" s="2">
         <v>329</v>
       </c>
@@ -19432,7 +19456,7 @@
       </c>
       <c r="L330" s="2"/>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A331" s="2">
         <v>330</v>
       </c>
@@ -19468,7 +19492,7 @@
       </c>
       <c r="L331" s="2"/>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A332" s="2">
         <v>331</v>
       </c>
@@ -19504,7 +19528,7 @@
       </c>
       <c r="L332" s="2"/>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A333" s="2">
         <v>332</v>
       </c>
@@ -19540,7 +19564,7 @@
       </c>
       <c r="L333" s="2"/>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A334" s="2">
         <v>333</v>
       </c>
@@ -19576,7 +19600,7 @@
       </c>
       <c r="L334" s="2"/>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A335" s="2">
         <v>334</v>
       </c>
@@ -19612,7 +19636,7 @@
       </c>
       <c r="L335" s="2"/>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A336" s="2">
         <v>335</v>
       </c>
@@ -19648,7 +19672,7 @@
       </c>
       <c r="L336" s="2"/>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A337" s="2">
         <v>336</v>
       </c>
@@ -19684,7 +19708,7 @@
       </c>
       <c r="L337" s="2"/>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A338" s="2">
         <v>337</v>
       </c>
@@ -19720,7 +19744,7 @@
       </c>
       <c r="L338" s="2"/>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A339" s="2">
         <v>338</v>
       </c>
@@ -19756,7 +19780,7 @@
       </c>
       <c r="L339" s="2"/>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A340" s="2">
         <v>339</v>
       </c>
@@ -19792,7 +19816,7 @@
       </c>
       <c r="L340" s="2"/>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A341" s="2">
         <v>340</v>
       </c>
@@ -19828,7 +19852,7 @@
       </c>
       <c r="L341" s="2"/>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A342" s="2">
         <v>341</v>
       </c>
@@ -19864,7 +19888,7 @@
       </c>
       <c r="L342" s="2"/>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A343" s="2">
         <v>342</v>
       </c>
@@ -19900,7 +19924,7 @@
       </c>
       <c r="L343" s="2"/>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A344" s="2">
         <v>343</v>
       </c>
@@ -19936,7 +19960,7 @@
       </c>
       <c r="L344" s="2"/>
     </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A345" s="2">
         <v>344</v>
       </c>
@@ -19972,7 +19996,7 @@
       </c>
       <c r="L345" s="2"/>
     </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A346" s="2">
         <v>345</v>
       </c>
@@ -20008,7 +20032,7 @@
       </c>
       <c r="L346" s="2"/>
     </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A347" s="2">
         <v>346</v>
       </c>
@@ -20044,7 +20068,7 @@
       </c>
       <c r="L347" s="2"/>
     </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A348" s="2">
         <v>347</v>
       </c>
@@ -20080,7 +20104,7 @@
       </c>
       <c r="L348" s="2"/>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A349" s="2">
         <v>348</v>
       </c>
@@ -20116,7 +20140,7 @@
       </c>
       <c r="L349" s="2"/>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A350" s="2">
         <v>349</v>
       </c>
@@ -20152,7 +20176,7 @@
       </c>
       <c r="L350" s="2"/>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A351" s="2">
         <v>350</v>
       </c>
@@ -20188,7 +20212,7 @@
       </c>
       <c r="L351" s="2"/>
     </row>
-    <row r="352" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A352" s="2">
         <v>351</v>
       </c>
@@ -20224,7 +20248,7 @@
       </c>
       <c r="L352" s="2"/>
     </row>
-    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A353" s="2">
         <v>352</v>
       </c>
@@ -20260,7 +20284,7 @@
       </c>
       <c r="L353" s="2"/>
     </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A354" s="2">
         <v>353</v>
       </c>
@@ -20296,7 +20320,7 @@
       </c>
       <c r="L354" s="2"/>
     </row>
-    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A355" s="2">
         <v>354</v>
       </c>
@@ -20332,7 +20356,7 @@
       </c>
       <c r="L355" s="2"/>
     </row>
-    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A356" s="2">
         <v>355</v>
       </c>
@@ -20368,7 +20392,7 @@
       </c>
       <c r="L356" s="2"/>
     </row>
-    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A357" s="2">
         <v>356</v>
       </c>
@@ -20404,7 +20428,7 @@
       </c>
       <c r="L357" s="2"/>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A358" s="2">
         <v>357</v>
       </c>
@@ -20440,7 +20464,7 @@
       </c>
       <c r="L358" s="2"/>
     </row>
-    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A359" s="2">
         <v>358</v>
       </c>
@@ -20476,7 +20500,7 @@
       </c>
       <c r="L359" s="2"/>
     </row>
-    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A360" s="2">
         <v>359</v>
       </c>
@@ -20512,7 +20536,7 @@
       </c>
       <c r="L360" s="2"/>
     </row>
-    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A361" s="2">
         <v>360</v>
       </c>
@@ -20548,7 +20572,7 @@
       </c>
       <c r="L361" s="2"/>
     </row>
-    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A362" s="2">
         <v>361</v>
       </c>
@@ -20584,7 +20608,7 @@
       </c>
       <c r="L362" s="2"/>
     </row>
-    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A363" s="2">
         <v>362</v>
       </c>
@@ -20620,7 +20644,7 @@
       </c>
       <c r="L363" s="2"/>
     </row>
-    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A364" s="2">
         <v>363</v>
       </c>
@@ -20656,7 +20680,7 @@
       </c>
       <c r="L364" s="2"/>
     </row>
-    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A365" s="2">
         <v>364</v>
       </c>
@@ -20692,7 +20716,7 @@
       </c>
       <c r="L365" s="2"/>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A366" s="2">
         <v>365</v>
       </c>
@@ -20728,7 +20752,7 @@
       </c>
       <c r="L366" s="2"/>
     </row>
-    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A367" s="2">
         <v>366</v>
       </c>
@@ -20764,7 +20788,7 @@
       </c>
       <c r="L367" s="2"/>
     </row>
-    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A368" s="2">
         <v>367</v>
       </c>
@@ -20800,7 +20824,7 @@
       </c>
       <c r="L368" s="2"/>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A369" s="2">
         <v>368</v>
       </c>
@@ -20836,7 +20860,7 @@
       </c>
       <c r="L369" s="2"/>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A370" s="2">
         <v>369</v>
       </c>
@@ -20872,7 +20896,7 @@
       </c>
       <c r="L370" s="2"/>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A371" s="2">
         <v>370</v>
       </c>
@@ -20908,7 +20932,7 @@
       </c>
       <c r="L371" s="2"/>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A372" s="2">
         <v>371</v>
       </c>
@@ -20944,7 +20968,7 @@
       </c>
       <c r="L372" s="2"/>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A373" s="2">
         <v>372</v>
       </c>
@@ -20980,7 +21004,7 @@
       </c>
       <c r="L373" s="2"/>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A374" s="2">
         <v>373</v>
       </c>
@@ -21016,7 +21040,7 @@
       </c>
       <c r="L374" s="2"/>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A375" s="2">
         <v>374</v>
       </c>
@@ -21052,7 +21076,7 @@
       </c>
       <c r="L375" s="2"/>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A376" s="2">
         <v>375</v>
       </c>
@@ -21088,7 +21112,7 @@
       </c>
       <c r="L376" s="2"/>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A377" s="2">
         <v>376</v>
       </c>
@@ -21124,7 +21148,7 @@
       </c>
       <c r="L377" s="2"/>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A378" s="2">
         <v>377</v>
       </c>
@@ -21160,7 +21184,7 @@
       </c>
       <c r="L378" s="2"/>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A379" s="2">
         <v>378</v>
       </c>
@@ -21196,7 +21220,7 @@
       </c>
       <c r="L379" s="2"/>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A380" s="2">
         <v>379</v>
       </c>
@@ -21232,7 +21256,7 @@
       </c>
       <c r="L380" s="2"/>
     </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A381" s="2">
         <v>380</v>
       </c>
@@ -21268,7 +21292,7 @@
       </c>
       <c r="L381" s="2"/>
     </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A382" s="2">
         <v>381</v>
       </c>
@@ -21304,7 +21328,7 @@
       </c>
       <c r="L382" s="2"/>
     </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A383" s="2">
         <v>382</v>
       </c>
@@ -21340,7 +21364,7 @@
       </c>
       <c r="L383" s="2"/>
     </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A384" s="2">
         <v>383</v>
       </c>
@@ -21376,7 +21400,7 @@
       </c>
       <c r="L384" s="2"/>
     </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A385" s="2">
         <v>384</v>
       </c>
@@ -21412,7 +21436,7 @@
       </c>
       <c r="L385" s="2"/>
     </row>
-    <row r="386" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A386" s="2">
         <v>385</v>
       </c>
@@ -21448,7 +21472,7 @@
       </c>
       <c r="L386" s="2"/>
     </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A387" s="2">
         <v>386</v>
       </c>
@@ -21484,7 +21508,7 @@
       </c>
       <c r="L387" s="2"/>
     </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A388" s="2">
         <v>387</v>
       </c>
@@ -21520,7 +21544,7 @@
       </c>
       <c r="L388" s="2"/>
     </row>
-    <row r="389" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A389" s="2">
         <v>388</v>
       </c>
@@ -21556,7 +21580,7 @@
       </c>
       <c r="L389" s="2"/>
     </row>
-    <row r="390" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A390" s="2">
         <v>389</v>
       </c>
@@ -21592,7 +21616,7 @@
       </c>
       <c r="L390" s="2"/>
     </row>
-    <row r="391" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A391" s="2">
         <v>390</v>
       </c>
@@ -21628,7 +21652,7 @@
       </c>
       <c r="L391" s="2"/>
     </row>
-    <row r="392" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A392" s="2">
         <v>391</v>
       </c>
@@ -21664,7 +21688,7 @@
       </c>
       <c r="L392" s="2"/>
     </row>
-    <row r="393" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A393" s="2">
         <v>392</v>
       </c>
@@ -21700,7 +21724,7 @@
       </c>
       <c r="L393" s="2"/>
     </row>
-    <row r="394" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A394" s="2">
         <v>393</v>
       </c>
@@ -21736,7 +21760,7 @@
       </c>
       <c r="L394" s="2"/>
     </row>
-    <row r="395" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A395" s="2">
         <v>394</v>
       </c>
@@ -21772,7 +21796,7 @@
       </c>
       <c r="L395" s="2"/>
     </row>
-    <row r="396" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A396" s="2">
         <v>395</v>
       </c>
@@ -21808,7 +21832,7 @@
       </c>
       <c r="L396" s="2"/>
     </row>
-    <row r="397" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A397" s="2">
         <v>396</v>
       </c>
@@ -21844,7 +21868,7 @@
       </c>
       <c r="L397" s="2"/>
     </row>
-    <row r="398" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A398" s="2">
         <v>397</v>
       </c>
@@ -21880,7 +21904,7 @@
       </c>
       <c r="L398" s="2"/>
     </row>
-    <row r="399" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A399" s="2">
         <v>398</v>
       </c>
@@ -21916,7 +21940,7 @@
       </c>
       <c r="L399" s="2"/>
     </row>
-    <row r="400" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A400" s="2">
         <v>399</v>
       </c>
@@ -21952,7 +21976,7 @@
       </c>
       <c r="L400" s="2"/>
     </row>
-    <row r="401" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A401" s="2">
         <v>400</v>
       </c>
@@ -21987,6 +22011,146 @@
         <v>2380</v>
       </c>
       <c r="L401" s="2"/>
+    </row>
+    <row r="402" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A402" s="2">
+        <v>401</v>
+      </c>
+      <c r="B402" s="2" t="s">
+        <v>2381</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>2382</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="E402" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F402" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G402" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H402" s="2" t="s">
+        <v>1579</v>
+      </c>
+      <c r="I402" s="2" t="s">
+        <v>1580</v>
+      </c>
+      <c r="J402" s="2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="K402" s="2" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="403" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A403" s="2">
+        <v>402</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>2383</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>2384</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="E403" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F403" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G403" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H403" s="2" t="s">
+        <v>1579</v>
+      </c>
+      <c r="I403" s="2" t="s">
+        <v>1580</v>
+      </c>
+      <c r="J403" s="2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="K403" s="2" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="404" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A404" s="2">
+        <v>403</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>2385</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>2387</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="E404" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F404" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G404" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H404" s="2" t="s">
+        <v>1579</v>
+      </c>
+      <c r="I404" s="2" t="s">
+        <v>1580</v>
+      </c>
+      <c r="J404" s="2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="K404" s="2" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="405" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A405" s="2">
+        <v>404</v>
+      </c>
+      <c r="B405" s="2" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="E405" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F405" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G405" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H405" s="2" t="s">
+        <v>1579</v>
+      </c>
+      <c r="I405" s="2" t="s">
+        <v>1580</v>
+      </c>
+      <c r="J405" s="2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="K405" s="2" t="s">
+        <v>2380</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>